<commit_message>
update weekly meeting minutes
</commit_message>
<xml_diff>
--- a/weeklyreport/FW5_Subteam2-Weekly_Meeting_Minutes.xlsx
+++ b/weeklyreport/FW5_Subteam2-Weekly_Meeting_Minutes.xlsx
@@ -25,22 +25,23 @@
     <sheet name="WK1507(draft)" sheetId="23" r:id="rId16"/>
     <sheet name="WK1529" sheetId="26" r:id="rId17"/>
     <sheet name="WK1530" sheetId="29" r:id="rId18"/>
-    <sheet name="WK1531(draft)" sheetId="31" r:id="rId19"/>
-    <sheet name="Status Review" sheetId="28" r:id="rId20"/>
-    <sheet name="Action Items" sheetId="1" r:id="rId21"/>
-    <sheet name="Media Strategy" sheetId="27" r:id="rId22"/>
-    <sheet name="WWWTL" sheetId="30" r:id="rId23"/>
+    <sheet name="WK1531" sheetId="31" r:id="rId19"/>
+    <sheet name="WK1532(draft)" sheetId="32" r:id="rId20"/>
+    <sheet name="Status Review" sheetId="28" r:id="rId21"/>
+    <sheet name="Action Items" sheetId="1" r:id="rId22"/>
+    <sheet name="Media Strategy" sheetId="27" r:id="rId23"/>
+    <sheet name="WWWTL" sheetId="30" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'Action Items'!$D$7:$J$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'Media Strategy'!$B$11:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'Action Items'!$D$7:$J$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'Media Strategy'!$B$11:$F$11</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="370">
   <si>
     <t>yachao</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1290,10 +1291,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Status Review</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Xiangbin.Feng</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1303,10 +1300,6 @@
   </si>
   <si>
     <t>Jiesen.Chen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Changfa.Huang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1506,10 +1499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>How to use CMPB for MSAF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Youming.Huang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1523,10 +1512,6 @@
   </si>
   <si>
     <t>Close all FB3-FFC items</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WK1530</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1769,10 +1754,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cmpb and exo's api cannot adjust to CB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Youming.Huang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1801,10 +1782,6 @@
   </si>
   <si>
     <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1819,11 +1796,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>check video freeze issue on U+
-???</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>check MRC with Jie.Zhang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1834,10 +1806,6 @@
   <si>
     <t xml:space="preserve">update "Status Review"
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>schedule a plan for leaning mediaplayer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1858,59 +1826,12 @@
   </si>
   <si>
     <t xml:space="preserve">[2015/7/24]
-initial
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[2015/7/24]
-confirm with Changfa &amp; Navy
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[2015/7/24]
 need architect help to confirm
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">[2015/7/24]
-initial
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Xiangbin.feng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helper of CB (FB2 FFC item)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[2015/7/24]
-继续准备
-[2015/7/17]
-资料收集,准备中
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[2015/7/24]
-amid MTK
-[2015/7/17]
-confirm with MTK
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[2015/7/24]
-continue to push
-[2015/7/17]
-check completed, not all items closed.
-Continue to review at next weekly meeting
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2092,7 +2013,310 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Executing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>handle MTK release plan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Youming.Huang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/27]
+initial
+FB2(WK26):
+For USB case, the MKV/WEBM, ASF/WMV, FLV, MP4, AVI, OGG/OGM, TS,PS  are support by now.
+For streaming:
+Protocol: DASH (single file single track), MSSS (single file single track), HLS
+•Java Extractor: Fragmented MP4 (single file single track), WebM (single file single track), TS for HLS
+FB3(WK2630):
+codec support: MP3,AMR,AWB,AAC,DTS,WAV,PCM,LPCM,FLAC,VORBIS
+trick APIs define (only API), 
+audio select APIs define(only API)
+external subtitle APIs define(only API).
+FB4(WK34):
+All codec
+trick 
+audio select
+external subtitle.
+DRM
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmpb and exo's api cannot adjust to CB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WK1531</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle FB3 FFC items
+Handle Action items
+Do a presentation on "C/C++ point"
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup MediaPlayerAdapter framework.
+Help youming integrate mtkmediaplayerwrapper into mediaplayeradapter.
+Learn and modify code of seamless playback demo app.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WK1530</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check video freeze issue on U+
+prepare seamless playback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add cmpb to media player framework
+2. Trace the MRC can’t play
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Debug the related issues about TS file play via CMPB
+2. Help to trace the MRC problem
+3. Debug the EU bugs
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the related MRC UI item.
+Fix some playback issue of DMR.
+Read the specifications of MRC XRS and DLNA Guidelines Working Draft 2014.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the FFC item.  
+Study the exoplayer library how to use mediacodec
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">needs MTK provide the support of DTS codec
+-&gt; track item_23
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DLNA,MRC has delayed for 1~2 weeks.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Debug bugs for U/U+ platform;
+2. Continue to learn the knowledge of seamless and example of seamless.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check video freeze issue on U+.
+2. Learning multimedia Framework knowledge
+3. Study and discuss the design and example of seamless playback[10%].
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期: 2015-07-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出席人数:  7 / 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>depend on exo trick API (provided by MTK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Study ContentExplorer app source code
+check FB3 FFC item about PTA
+use media-adpter to replace mediaplayer(java)  (do a test)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/07/31]
+have done a presentation
+[2015/7/24]
+继续准备
+[2015/7/17]
+资料收集,准备中
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helper of CB (FB2 FFC item)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+continue to track
+[2015/7/24]
+initial
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+there still has 10+ items alive(need ation!)
+[2015/7/24]
+continue to push
+[2015/7/17]
+check completed, not all items closed.
+Continue to review at next weekly meeting
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+have done a presentation
+[2015/7/24]
+initial
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use cmpb to playback ts file on MSAF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+close this item as item_18 handled the same issue.
+[2015/7/24]
+initial
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+at this time, we should focus on media framework.
+And in next 3 weeks, changfa will handle the gstream issue.
+so, pending this item.
+[2015/7/24]
+confirm with Changfa &amp; Navy
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[2015/7/31]
+there are 2 cmpb class in jave layer,
+the one is derived from mediaplayer class,
+the other is NOT.
+We will try to use the first one.
+Lower the priority.
+[2015/7/24]
+amid MTK
+[2015/7/17]
+confirm with MTK
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">外派參加訓練或研討會後,請務必將邀請函/會議通知/會議資料/相片等材料,發送给Andy
+所有專利申請的駁回申述,务必跟主管討論後,統一由專利窗口Tini或Andy通知事務所.尤其是歐美日的專利
+离职需通过OA提交离职申请,处理周期为1个月
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">更新 Status Review
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">min 分享了 C/C++ 指针 相关知识.
+xiangbin 分享了 Media Framework 相关知识, 描述了media framework的轮廓
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disscus mediaplayer framework
+need support the following state:
+1.native media app with mediaplayer-class
+2.native media app with exo-class
+3.3rd media app with mediaplayer-class
+4.3rd media app with exo-class
+5.all media app with ts format</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Min.Lee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2015/7/31]
+initial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">讨论了现有 mediaplayer framework 对媒体文件的播放支持(电视原生应用_mediaplayer,电视原生应用_exo,第三方应用_mediaplaeyr,第三方应用_exo,ts!!文件播放), 设定为下周中间解决问题!!! 建立item_27用于追踪
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.handle a meeting to disscus medipalyer framework
+2.Handle FB3 FFC items
+3.Handle Action items
+4.Prepare a presentation of Android-Binder
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Draw the flow from exo library to omx 
+2.Go on check the FFC item
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Check the related MRC playback function.
+2.Help to check the FFC item of Exposing USB states to DMC.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.discuss seamless with xiangbin
+2.discuss mediaplayer framwork with youming &amp; min
+3.discuss Gstreamer with changfa </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Study Gstream structure and usage(important!!, 3WKs)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">?2015/3/1起本市户籍人员失业保险个人缴费比例从1%调整为0.5%
+?2015/7/1起，所有正式工缴纳公积金比例由14%调整为16%(单位&amp;个人各承担8%)
+?2015/8/4起，公司公积金开户行由原来新店建行转移至火炬园支行
+?在得知需要出差时就及时尽快在E-Flow系统中提出差申请,否则会影响签证申请/机票出票等问题
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2103,7 +2327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2346,6 +2570,45 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2374,13 +2637,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2794,7 +3057,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2942,9 +3205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2981,9 +3241,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3029,7 +3286,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -3044,12 +3301,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3095,6 +3346,48 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3208,9 +3501,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4350,10 +4640,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="92.25">
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="105"/>
+      <c r="C2" s="115"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
@@ -4482,7 +4772,7 @@
         <v>155</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="94.5">
@@ -4490,7 +4780,7 @@
         <v>156</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="40.5">
@@ -4498,7 +4788,7 @@
         <v>166</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="2:3">
@@ -4528,7 +4818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C13"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4542,13 +4832,13 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="14.25" thickBot="1">
@@ -4567,7 +4857,7 @@
         <v>150</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="27">
@@ -4575,7 +4865,7 @@
         <v>155</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="67.5">
@@ -4583,7 +4873,7 @@
         <v>156</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="148.5">
@@ -4591,7 +4881,7 @@
         <v>166</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="2:3">
@@ -4599,7 +4889,7 @@
         <v>180</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="18.75" customHeight="1">
@@ -4619,10 +4909,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C14"/>
+  <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4633,80 +4923,75 @@
     <col min="4" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="31.5">
-      <c r="B2" s="138" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="2:3">
+      <c r="B3" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="14.25" thickBot="1">
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="2:3" ht="67.5">
-      <c r="B7" s="21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="14.25" thickBot="1">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="2:3" ht="67.5">
+      <c r="B6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C6" s="43" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="7" spans="2:3" ht="81">
+      <c r="B7" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="27">
       <c r="B8" s="10" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C8" s="44" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="54">
+      <c r="B9" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="40.5">
+      <c r="B10" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="148.5">
-      <c r="B11" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="18.75" customHeight="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="2:3" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B14" s="13"/>
-      <c r="C14" s="15"/>
+    <row r="12" spans="2:3" ht="18.75" customHeight="1">
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="2:3" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B13" s="13"/>
+      <c r="C13" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4759,10 +5044,10 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -4770,8 +5055,8 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="75" customHeight="1">
-      <c r="B9" s="102"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -4779,8 +5064,8 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1">
-      <c r="B10" s="102"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -4788,8 +5073,8 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" thickBot="1">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -4808,11 +5093,111 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E14"/>
+  <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9" style="7"/>
+    <col min="2" max="2" width="21.75" style="7" customWidth="1"/>
+    <col min="3" max="3" width="69.75" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="31.5">
+      <c r="B2" s="97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="14.25" thickBot="1">
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="2:3" ht="67.5">
+      <c r="B7" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="81">
+      <c r="B8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="148.5">
+      <c r="B11" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="18.75" customHeight="1">
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="2:3" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:E23"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4825,157 +5210,265 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="32.25" thickBot="1">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="116" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" s="116"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" customHeight="1">
+      <c r="B4" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="22.5" customHeight="1">
+      <c r="B5" s="101" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="100"/>
+    </row>
+    <row r="6" spans="2:5" ht="78.75">
+      <c r="B6" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="103" t="s">
+        <v>330</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>364</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="47.25">
+      <c r="B7" s="102" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>338</v>
+      </c>
+      <c r="D7" s="103" t="s">
+        <v>365</v>
+      </c>
+      <c r="E7" s="105"/>
+    </row>
+    <row r="8" spans="2:5" ht="78.75">
+      <c r="B8" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="106"/>
-    </row>
-    <row r="4" spans="2:5" ht="19.5" customHeight="1">
-      <c r="B4" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B5" s="62" t="s">
-        <v>240</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="49"/>
-    </row>
-    <row r="6" spans="2:5" ht="54">
-      <c r="B6" s="48" t="s">
+      <c r="C8" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="105"/>
+    </row>
+    <row r="9" spans="2:5" ht="63">
+      <c r="B9" s="102" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="103" t="s">
+        <v>335</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>336</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="78.75">
+      <c r="B10" s="102" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="104" t="s">
         <v>337</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="E6" s="49"/>
-    </row>
-    <row r="7" spans="2:5" ht="67.5">
-      <c r="B7" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="83" t="s">
-        <v>288</v>
-      </c>
-      <c r="D7" s="83" t="s">
-        <v>289</v>
-      </c>
-      <c r="E7" s="49"/>
-    </row>
-    <row r="8" spans="2:5" ht="54">
-      <c r="B8" s="48" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="83" t="s">
-        <v>326</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>301</v>
-      </c>
-      <c r="E8" s="49"/>
-    </row>
-    <row r="9" spans="2:5" ht="40.5">
-      <c r="B9" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="83" t="s">
-        <v>293</v>
-      </c>
-      <c r="D9" s="83" t="s">
-        <v>300</v>
-      </c>
-      <c r="E9" s="84" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="54">
-      <c r="B10" s="48" t="s">
+      <c r="D10" s="104" t="s">
+        <v>366</v>
+      </c>
+      <c r="E10" s="106" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="22.5" customHeight="1">
+      <c r="B11" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" s="107"/>
+      <c r="E11" s="105"/>
+    </row>
+    <row r="12" spans="2:5" ht="78.75">
+      <c r="B12" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="83" t="s">
-        <v>299</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="E10" s="84" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B11" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="49"/>
-    </row>
-    <row r="12" spans="2:5" ht="48" customHeight="1">
-      <c r="B12" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="C12" s="83" t="s">
-        <v>287</v>
-      </c>
-      <c r="D12" s="83" t="s">
-        <v>294</v>
-      </c>
-      <c r="E12" s="49"/>
-    </row>
-    <row r="13" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B13" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="49"/>
-    </row>
-    <row r="14" spans="2:5" ht="14.25" thickBot="1">
-      <c r="B14" s="107" t="s">
-        <v>218</v>
+      <c r="C12" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="D12" s="103" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="105"/>
+    </row>
+    <row r="13" spans="2:5" ht="63">
+      <c r="B13" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="103" t="s">
+        <v>346</v>
+      </c>
+      <c r="D13" s="109" t="s">
+        <v>368</v>
+      </c>
+      <c r="E13" s="105"/>
+    </row>
+    <row r="14" spans="2:5" ht="22.5" customHeight="1">
+      <c r="B14" s="101" t="s">
+        <v>332</v>
       </c>
       <c r="C14" s="108"/>
       <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
+      <c r="E14" s="105"/>
+    </row>
+    <row r="15" spans="2:5" ht="63">
+      <c r="B15" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="104" t="s">
+        <v>321</v>
+      </c>
+      <c r="D15" s="104" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" s="105"/>
+    </row>
+    <row r="16" spans="2:5" ht="78.75">
+      <c r="B16" s="102" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="105"/>
+    </row>
+    <row r="17" spans="2:5" ht="63">
+      <c r="B17" s="102" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="103" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>333</v>
+      </c>
+      <c r="E17" s="105"/>
+    </row>
+    <row r="18" spans="2:5" ht="47.25">
+      <c r="B18" s="102" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="103" t="s">
+        <v>288</v>
+      </c>
+      <c r="D18" s="103" t="s">
+        <v>294</v>
+      </c>
+      <c r="E18" s="106" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="63">
+      <c r="B19" s="102" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" s="104" t="s">
+        <v>295</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="22.5" customHeight="1">
+      <c r="B20" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="104" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="107"/>
+      <c r="E20" s="105"/>
+    </row>
+    <row r="21" spans="2:5" ht="48" customHeight="1">
+      <c r="B21" s="102" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="103" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="105"/>
+    </row>
+    <row r="22" spans="2:5" ht="22.5" customHeight="1">
+      <c r="B22" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="104" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="107"/>
+      <c r="E22" s="105"/>
+    </row>
+    <row r="23" spans="2:5" ht="14.25" thickBot="1">
+      <c r="B23" s="117" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4998,81 +5491,81 @@
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" thickBot="1"/>
     <row r="2" spans="1:13" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="125" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="117"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="127"/>
     </row>
     <row r="3" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A3" s="110"/>
-      <c r="B3" s="111" t="s">
+      <c r="A3" s="120"/>
+      <c r="B3" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="110"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="120"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A4" s="110"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="110"/>
+    <row r="4" spans="1:13" ht="5.25" customHeight="1" thickBot="1">
+      <c r="A4" s="120"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" ht="14.25" hidden="1" thickBot="1">
-      <c r="A5" s="110"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="110"/>
+      <c r="A5" s="120"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="120"/>
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" ht="14.25" hidden="1" customHeight="1" thickBot="1">
-      <c r="A6" s="110"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="110"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="120"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" ht="57" customHeight="1" thickBot="1">
-      <c r="A7" s="110"/>
+    <row r="7" spans="1:13" ht="72" customHeight="1" thickBot="1">
+      <c r="A7" s="120"/>
       <c r="B7" s="22" t="s">
         <v>16</v>
       </c>
@@ -5100,12 +5593,12 @@
       <c r="J7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="110"/>
+      <c r="K7" s="120"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" ht="148.5" hidden="1">
-      <c r="A8" s="110"/>
+    <row r="8" spans="1:13" ht="148.5">
+      <c r="A8" s="120"/>
       <c r="B8" s="19">
         <v>1</v>
       </c>
@@ -5133,12 +5626,12 @@
       <c r="J8" s="29">
         <v>41866</v>
       </c>
-      <c r="K8" s="110"/>
+      <c r="K8" s="120"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" ht="256.5" hidden="1">
-      <c r="A9" s="110"/>
+    <row r="9" spans="1:13" ht="256.5">
+      <c r="A9" s="120"/>
       <c r="B9" s="19">
         <v>2</v>
       </c>
@@ -5164,12 +5657,12 @@
       <c r="J9" s="29">
         <v>41866</v>
       </c>
-      <c r="K9" s="110"/>
+      <c r="K9" s="120"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" ht="94.5" hidden="1">
-      <c r="A10" s="110"/>
+    <row r="10" spans="1:13" ht="94.5">
+      <c r="A10" s="120"/>
       <c r="B10" s="19">
         <v>3</v>
       </c>
@@ -5195,12 +5688,12 @@
       <c r="J10" s="29">
         <v>41866</v>
       </c>
-      <c r="K10" s="110"/>
+      <c r="K10" s="120"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" ht="108" hidden="1">
-      <c r="A11" s="110"/>
+    <row r="11" spans="1:13" ht="108">
+      <c r="A11" s="120"/>
       <c r="B11" s="19">
         <v>4</v>
       </c>
@@ -5226,12 +5719,12 @@
       <c r="J11" s="29">
         <v>41866</v>
       </c>
-      <c r="K11" s="110"/>
+      <c r="K11" s="120"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" ht="108" hidden="1">
-      <c r="A12" s="110"/>
+    <row r="12" spans="1:13" ht="108">
+      <c r="A12" s="120"/>
       <c r="B12" s="19">
         <v>5</v>
       </c>
@@ -5255,12 +5748,12 @@
       <c r="J12" s="29">
         <v>41880</v>
       </c>
-      <c r="K12" s="110"/>
+      <c r="K12" s="120"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" ht="81" hidden="1">
-      <c r="A13" s="110"/>
+    <row r="13" spans="1:13" ht="81">
+      <c r="A13" s="120"/>
       <c r="B13" s="19">
         <v>6</v>
       </c>
@@ -5284,12 +5777,12 @@
       <c r="J13" s="29">
         <v>41880</v>
       </c>
-      <c r="K13" s="110"/>
+      <c r="K13" s="120"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" ht="40.5" hidden="1">
-      <c r="A14" s="110"/>
+    <row r="14" spans="1:13" ht="40.5">
+      <c r="A14" s="120"/>
       <c r="B14" s="19">
         <v>7</v>
       </c>
@@ -5313,12 +5806,12 @@
       <c r="J14" s="29">
         <v>41882</v>
       </c>
-      <c r="K14" s="110"/>
+      <c r="K14" s="120"/>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" ht="81" hidden="1">
-      <c r="A15" s="110"/>
+    <row r="15" spans="1:13" ht="81">
+      <c r="A15" s="120"/>
       <c r="B15" s="19">
         <v>8</v>
       </c>
@@ -5342,12 +5835,12 @@
       <c r="J15" s="29">
         <v>41936</v>
       </c>
-      <c r="K15" s="110"/>
+      <c r="K15" s="120"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" ht="81" hidden="1">
-      <c r="A16" s="110"/>
+    <row r="16" spans="1:13" ht="81">
+      <c r="A16" s="120"/>
       <c r="B16" s="19">
         <v>9</v>
       </c>
@@ -5365,18 +5858,18 @@
         <v>139</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="29">
         <v>42032</v>
       </c>
-      <c r="K16" s="110"/>
+      <c r="K16" s="120"/>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" ht="54" hidden="1">
-      <c r="A17" s="110"/>
+    <row r="17" spans="1:13" ht="54">
+      <c r="A17" s="120"/>
       <c r="B17" s="19">
         <v>10</v>
       </c>
@@ -5400,12 +5893,12 @@
       <c r="J17" s="29">
         <v>42032</v>
       </c>
-      <c r="K17" s="110"/>
+      <c r="K17" s="120"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="81" hidden="1">
-      <c r="A18" s="110"/>
+    <row r="18" spans="1:13" ht="81">
+      <c r="A18" s="120"/>
       <c r="B18" s="19">
         <v>11</v>
       </c>
@@ -5429,12 +5922,12 @@
       <c r="J18" s="29">
         <v>42032</v>
       </c>
-      <c r="K18" s="110"/>
+      <c r="K18" s="120"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" ht="108" hidden="1">
-      <c r="A19" s="110"/>
+    <row r="19" spans="1:13" ht="108">
+      <c r="A19" s="120"/>
       <c r="B19" s="19">
         <v>12</v>
       </c>
@@ -5452,7 +5945,7 @@
         <v>52</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I19" s="28" t="s">
         <v>168</v>
@@ -5460,12 +5953,12 @@
       <c r="J19" s="29">
         <v>42032</v>
       </c>
-      <c r="K19" s="110"/>
+      <c r="K19" s="120"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
     </row>
-    <row r="20" spans="1:13" ht="121.5">
-      <c r="A20" s="110"/>
+    <row r="20" spans="1:13" ht="66.75" customHeight="1">
+      <c r="A20" s="120"/>
       <c r="B20" s="19">
         <v>13</v>
       </c>
@@ -5483,20 +5976,20 @@
         <v>207</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="I20" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="J20" s="58">
+      <c r="J20" s="57">
         <v>42199</v>
       </c>
-      <c r="K20" s="110"/>
+      <c r="K20" s="120"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:13" ht="40.5" hidden="1">
-      <c r="A21" s="110"/>
+    <row r="21" spans="1:13" ht="40.5">
+      <c r="A21" s="120"/>
       <c r="B21" s="19">
         <v>14</v>
       </c>
@@ -5508,24 +6001,24 @@
         <v>49</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G21" s="38" t="s">
         <v>207</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I21" s="28"/>
-      <c r="J21" s="58">
+      <c r="J21" s="57">
         <v>42202</v>
       </c>
-      <c r="K21" s="110"/>
+      <c r="K21" s="120"/>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
     </row>
-    <row r="22" spans="1:13" ht="67.5" hidden="1">
-      <c r="A22" s="110"/>
+    <row r="22" spans="1:13" ht="67.5">
+      <c r="A22" s="120"/>
       <c r="B22" s="19">
         <v>15</v>
       </c>
@@ -5537,55 +6030,55 @@
         <v>34</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G22" s="38" t="s">
         <v>207</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="J22" s="58">
+        <v>220</v>
+      </c>
+      <c r="J22" s="57">
         <v>42202</v>
       </c>
-      <c r="K22" s="110"/>
+      <c r="K22" s="120"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
     </row>
-    <row r="23" spans="1:13" ht="67.5" hidden="1">
-      <c r="A23" s="110"/>
+    <row r="23" spans="1:13" ht="94.5">
+      <c r="A23" s="120"/>
       <c r="B23" s="19">
         <v>16</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="41" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E23" s="47" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="I23" s="28"/>
-      <c r="J23" s="58">
+      <c r="J23" s="57">
         <v>42202</v>
       </c>
-      <c r="K23" s="110"/>
+      <c r="K23" s="120"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
     </row>
-    <row r="24" spans="1:13" ht="67.5" hidden="1">
-      <c r="A24" s="110"/>
+    <row r="24" spans="1:13" ht="67.5">
+      <c r="A24" s="120"/>
       <c r="B24" s="19">
         <v>17</v>
       </c>
@@ -5597,24 +6090,24 @@
         <v>49</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="I24" s="28"/>
-      <c r="J24" s="58">
+      <c r="J24" s="57">
         <v>42202</v>
       </c>
-      <c r="K24" s="110"/>
+      <c r="K24" s="120"/>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
     </row>
-    <row r="25" spans="1:13" ht="67.5" hidden="1">
-      <c r="A25" s="110"/>
+    <row r="25" spans="1:13" ht="148.5">
+      <c r="A25" s="120"/>
       <c r="B25" s="19">
         <v>18</v>
       </c>
@@ -5623,330 +6116,348 @@
         <v>38</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>235</v>
+        <v>352</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="I25" s="28"/>
-      <c r="J25" s="58">
+      <c r="J25" s="57">
         <v>42202</v>
       </c>
-      <c r="K25" s="110"/>
+      <c r="K25" s="120"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
     </row>
-    <row r="26" spans="1:13" ht="81">
-      <c r="A26" s="110"/>
+    <row r="26" spans="1:13" ht="108">
+      <c r="A26" s="120"/>
       <c r="B26" s="19">
         <v>19</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="41" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G26" s="38" t="s">
         <v>207</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>316</v>
+        <v>350</v>
       </c>
       <c r="I26" s="28"/>
-      <c r="J26" s="58">
+      <c r="J26" s="57">
         <v>42202</v>
       </c>
-      <c r="K26" s="110"/>
+      <c r="K26" s="120"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
     </row>
-    <row r="27" spans="1:13" ht="40.5" hidden="1">
-      <c r="A27" s="110"/>
+    <row r="27" spans="1:13" ht="67.5">
+      <c r="A27" s="120"/>
       <c r="B27" s="19">
         <v>20</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="61" t="s">
         <v>32</v>
       </c>
       <c r="F27" s="36" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="I27" s="28"/>
-      <c r="J27" s="58">
+      <c r="J27" s="57">
         <v>42209</v>
       </c>
-      <c r="K27" s="110"/>
+      <c r="K27" s="120"/>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
     </row>
-    <row r="28" spans="1:13" ht="40.5" hidden="1">
-      <c r="A28" s="110"/>
+    <row r="28" spans="1:13" ht="108">
+      <c r="A28" s="120"/>
       <c r="B28" s="19">
         <v>21</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="61" t="s">
         <v>32</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
       <c r="I28" s="28"/>
-      <c r="J28" s="58">
+      <c r="J28" s="57">
         <v>42209</v>
       </c>
-      <c r="K28" s="110"/>
+      <c r="K28" s="120"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
     </row>
-    <row r="29" spans="1:13" ht="40.5" hidden="1">
-      <c r="A29" s="110"/>
+    <row r="29" spans="1:13" ht="40.5">
+      <c r="A29" s="120"/>
       <c r="B29" s="19">
         <v>22</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="41" t="s">
-        <v>296</v>
-      </c>
-      <c r="E29" s="63" t="s">
-        <v>297</v>
+        <v>291</v>
+      </c>
+      <c r="E29" s="61" t="s">
+        <v>292</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I29" s="28"/>
-      <c r="J29" s="58">
+      <c r="J29" s="57">
         <v>42209</v>
       </c>
-      <c r="K29" s="110"/>
+      <c r="K29" s="120"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
     </row>
-    <row r="30" spans="1:13" ht="40.5">
-      <c r="A30" s="110"/>
+    <row r="30" spans="1:13" ht="67.5">
+      <c r="A30" s="120"/>
       <c r="B30" s="19">
         <v>23</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="G30" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="E30" s="63" t="s">
-        <v>297</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>303</v>
-      </c>
       <c r="H30" s="28" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="I30" s="28"/>
-      <c r="J30" s="58">
+      <c r="J30" s="57">
         <v>42209</v>
       </c>
-      <c r="K30" s="110"/>
+      <c r="K30" s="120"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
     </row>
-    <row r="31" spans="1:13" ht="40.5">
-      <c r="A31" s="110"/>
+    <row r="31" spans="1:13" ht="67.5">
+      <c r="A31" s="120"/>
       <c r="B31" s="19">
         <v>24</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>34</v>
+        <v>291</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>292</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>305</v>
+        <v>348</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="I31" s="28"/>
-      <c r="J31" s="58">
+      <c r="J31" s="57">
         <v>42209</v>
       </c>
-      <c r="K31" s="110"/>
+      <c r="K31" s="120"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
     </row>
-    <row r="32" spans="1:13" ht="40.5" hidden="1">
-      <c r="A32" s="110"/>
+    <row r="32" spans="1:13" ht="67.5">
+      <c r="A32" s="120"/>
       <c r="B32" s="19">
         <v>25</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="41" t="s">
-        <v>296</v>
-      </c>
-      <c r="E32" s="63" t="s">
-        <v>297</v>
+        <v>86</v>
+      </c>
+      <c r="E32" s="78" t="s">
+        <v>317</v>
       </c>
       <c r="F32" s="36" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>311</v>
+        <v>351</v>
       </c>
       <c r="I32" s="28"/>
-      <c r="J32" s="58">
+      <c r="J32" s="57">
         <v>42209</v>
       </c>
-      <c r="K32" s="110"/>
+      <c r="K32" s="120"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
     </row>
-    <row r="33" spans="1:15" ht="40.5">
-      <c r="A33" s="110"/>
+    <row r="33" spans="1:15" ht="69" customHeight="1">
+      <c r="A33" s="120"/>
       <c r="B33" s="19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="80" t="s">
-        <v>332</v>
+        <v>322</v>
+      </c>
+      <c r="E33" s="96" t="s">
+        <v>323</v>
       </c>
       <c r="F33" s="36" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="I33" s="28"/>
-      <c r="J33" s="58">
-        <v>42209</v>
-      </c>
-      <c r="K33" s="110"/>
+      <c r="J33" s="57">
+        <v>42212</v>
+      </c>
+      <c r="K33" s="120"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
     </row>
-    <row r="34" spans="1:15" ht="42" customHeight="1" thickBot="1">
-      <c r="A34" s="110"/>
-      <c r="B34" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="119"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="122"/>
-      <c r="K34" s="110"/>
+    <row r="34" spans="1:15" ht="108">
+      <c r="A34" s="120"/>
+      <c r="B34" s="19">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="98" t="s">
+        <v>359</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="57">
+        <v>42216</v>
+      </c>
+      <c r="K34" s="120"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
     </row>
-    <row r="35" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A35" s="110"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="110"/>
+    <row r="35" spans="1:15" ht="42" customHeight="1" thickBot="1">
+      <c r="A35" s="120"/>
+      <c r="B35" s="128">
+        <f>COUNT(B8:B34)</f>
+        <v>27</v>
+      </c>
+      <c r="C35" s="129"/>
+      <c r="D35" s="130"/>
+      <c r="E35" s="131"/>
+      <c r="F35" s="131"/>
+      <c r="G35" s="131"/>
+      <c r="H35" s="131"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="132"/>
+      <c r="K35" s="120"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A36" s="110"/>
-      <c r="B36" s="113"/>
-      <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="113"/>
-      <c r="G36" s="113"/>
-      <c r="H36" s="113"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="110"/>
+      <c r="A36" s="120"/>
+      <c r="B36" s="123"/>
+      <c r="C36" s="124"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="123"/>
+      <c r="I36" s="123"/>
+      <c r="J36" s="123"/>
+      <c r="K36" s="120"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A37" s="110"/>
-      <c r="B37" s="113"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="113"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="113"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="113"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="113"/>
-      <c r="K37" s="110"/>
+      <c r="A37" s="120"/>
+      <c r="B37" s="123"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="123"/>
+      <c r="I37" s="123"/>
+      <c r="J37" s="123"/>
+      <c r="K37" s="120"/>
       <c r="L37" s="18"/>
       <c r="M37" s="18"/>
     </row>
-    <row r="38" spans="1:15">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+    <row r="38" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A38" s="120"/>
+      <c r="B38" s="123"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="123"/>
+      <c r="K38" s="120"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
     </row>
     <row r="39" spans="1:15">
       <c r="B39" s="1"/>
@@ -5960,7 +6471,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" thickBot="1">
+    <row r="40" spans="1:15">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -5972,133 +6483,137 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:15">
-      <c r="M41" s="4" t="s">
+    <row r="41" spans="1:15" ht="14.25" thickBot="1">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="M42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N41" s="30" t="s">
+      <c r="N42" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="O41" s="31" t="s">
+      <c r="O42" s="31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
-      <c r="M42" s="5"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="32"/>
-    </row>
     <row r="43" spans="1:15">
-      <c r="M43" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O43" s="32" t="s">
-        <v>54</v>
-      </c>
+      <c r="M43" s="5"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="32"/>
     </row>
     <row r="44" spans="1:15">
       <c r="M44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="M45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="32" t="s">
+      <c r="O45" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="14.25" thickBot="1">
-      <c r="M45" s="5" t="s">
+    <row r="46" spans="1:15" ht="14.25" thickBot="1">
+      <c r="M46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O45" s="32" t="s">
+      <c r="O46" s="32" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="M46" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O46" s="32" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="M47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O47" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="M48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O47" s="32" t="s">
+      <c r="O48" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="14.25" thickBot="1">
-      <c r="M48" s="6" t="s">
+    <row r="49" spans="13:15" ht="14.25" thickBot="1">
+      <c r="M49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O48" s="32" t="s">
+      <c r="O49" s="32" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="13:15">
-      <c r="M49" s="34"/>
-      <c r="O49" s="32" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="50" spans="13:15">
       <c r="M50" s="34"/>
       <c r="O50" s="32" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="13:15">
       <c r="M51" s="34"/>
       <c r="O51" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="13:15" ht="14.25" thickBot="1">
-      <c r="O52" s="33" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="13:15">
+      <c r="M52" s="34"/>
+      <c r="O52" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="13:15" ht="14.25" thickBot="1">
+      <c r="O53" s="33" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D7:J34">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="Executing"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="Min.Lee"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="D7:J35">
+    <filterColumn colId="0"/>
+    <filterColumn colId="3"/>
   </autoFilter>
   <mergeCells count="6">
-    <mergeCell ref="K3:K37"/>
+    <mergeCell ref="K3:K38"/>
     <mergeCell ref="B3:J6"/>
-    <mergeCell ref="B35:J37"/>
-    <mergeCell ref="A3:A37"/>
+    <mergeCell ref="B36:J38"/>
+    <mergeCell ref="A3:A38"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E38:E40 D8:D33">
-      <formula1>$M$42:$M$48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39:E41 D8:D34">
+      <formula1>$M$43:$M$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E33">
-      <formula1>$N$42:$N$45</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E34">
+      <formula1>$N$43:$N$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G33">
-      <formula1>$O$42:$O$52</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G34">
+      <formula1>$O$43:$O$53</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6106,12 +6621,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6132,192 +6647,192 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="B2" s="133" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
+      <c r="B2" s="143" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="133" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
+      <c r="B3" s="143" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
     </row>
     <row r="4" spans="1:18" ht="32.25" thickBot="1">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="116" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
     </row>
     <row r="5" spans="1:18" ht="13.5" customHeight="1">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="134" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="136"/>
     </row>
     <row r="6" spans="1:18" ht="13.5" customHeight="1">
-      <c r="B6" s="127"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="129"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="139"/>
     </row>
     <row r="7" spans="1:18" ht="13.5" customHeight="1">
-      <c r="B7" s="127"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="129"/>
+      <c r="B7" s="137"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="139"/>
     </row>
     <row r="8" spans="1:18" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B8" s="130"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="142"/>
     </row>
     <row r="10" spans="1:18" ht="23.25" thickBot="1">
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="133" t="s">
         <v>184</v>
       </c>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
       <c r="G10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I10" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M10" t="s">
+        <v>269</v>
+      </c>
+      <c r="O10" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="14.25" thickBot="1">
+      <c r="B11" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H11" s="63" t="s">
         <v>273</v>
       </c>
-      <c r="O10" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="14.25" thickBot="1">
-      <c r="B11" s="54" t="s">
-        <v>202</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>205</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="H11" s="65" t="s">
-        <v>277</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="J11" s="65" t="s">
-        <v>277</v>
-      </c>
-      <c r="K11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="L11" s="65" t="s">
-        <v>277</v>
-      </c>
-      <c r="M11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="N11" s="65" t="s">
-        <v>277</v>
-      </c>
-      <c r="O11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="P11" s="65" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q11" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="R11" s="65" t="s">
-        <v>277</v>
+      <c r="I11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="J11" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="O11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="P11" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q11" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="R11" s="63" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="14.25">
-      <c r="A12" s="78"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="C12" s="94" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="87">
+      <c r="C12" s="90" t="s">
+        <v>302</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="83">
         <f>AVERAGE(G12,I12,K12,M12,O12,Q12)</f>
         <v>7.75</v>
       </c>
-      <c r="F12" s="96">
+      <c r="F12" s="92">
         <f>AVERAGE(E12,H12,J12,L12,N12,P12,R12)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="G12" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="H12" s="68" t="s">
-        <v>242</v>
-      </c>
-      <c r="I12" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="J12" s="68" t="s">
-        <v>251</v>
-      </c>
-      <c r="K12" s="66">
+      <c r="G12" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="K12" s="64">
         <v>9</v>
       </c>
-      <c r="L12" s="68">
+      <c r="L12" s="66">
         <v>9</v>
       </c>
-      <c r="M12" s="70">
+      <c r="M12" s="68">
         <v>9</v>
       </c>
-      <c r="N12" s="68">
+      <c r="N12" s="66">
         <v>9</v>
       </c>
-      <c r="O12" s="66">
+      <c r="O12" s="64">
         <v>6</v>
       </c>
-      <c r="P12" s="68">
+      <c r="P12" s="66">
         <v>9</v>
       </c>
-      <c r="Q12" s="74">
+      <c r="Q12" s="72">
         <v>7</v>
       </c>
-      <c r="R12" s="75">
+      <c r="R12" s="73">
         <v>8</v>
       </c>
     </row>
@@ -6326,309 +6841,309 @@
       <c r="C13" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="E13" s="87">
+      <c r="E13" s="83">
         <f t="shared" ref="E13:E25" si="0">AVERAGE(G13,I13,K13,M13,O13,Q13)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="F13" s="85">
+      <c r="F13" s="81">
         <f>AVERAGE(E13,H13,J13,L13,N13,P13,R13)</f>
         <v>6.4444444444444455</v>
       </c>
-      <c r="G13" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="H13" s="68">
+      <c r="G13" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" s="66">
         <v>5</v>
       </c>
-      <c r="I13" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="J13" s="68">
+      <c r="I13" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="J13" s="66">
         <v>5</v>
       </c>
-      <c r="K13" s="66">
+      <c r="K13" s="64">
         <v>7</v>
       </c>
-      <c r="L13" s="68">
+      <c r="L13" s="66">
         <v>7</v>
       </c>
-      <c r="M13" s="70" t="s">
-        <v>258</v>
-      </c>
-      <c r="N13" s="71" t="s">
-        <v>259</v>
-      </c>
-      <c r="O13" s="66">
+      <c r="M13" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="N13" s="69" t="s">
+        <v>255</v>
+      </c>
+      <c r="O13" s="64">
         <v>7</v>
       </c>
-      <c r="P13" s="68">
+      <c r="P13" s="66">
         <v>8</v>
       </c>
-      <c r="Q13" s="74">
+      <c r="Q13" s="72">
         <v>6</v>
       </c>
-      <c r="R13" s="75">
+      <c r="R13" s="73">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="14.25">
       <c r="B14" s="48"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="83">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="F14" s="85">
+      <c r="F14" s="81">
         <f t="shared" ref="F14:F25" si="1">AVERAGE(E14,H14,J14,L14,N14,P14,R14)</f>
         <v>6.4444444444444455</v>
       </c>
-      <c r="G14" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="H14" s="68">
+      <c r="G14" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" s="66">
         <v>5</v>
       </c>
-      <c r="I14" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="J14" s="68">
+      <c r="I14" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" s="66">
         <v>5</v>
       </c>
-      <c r="K14" s="66">
+      <c r="K14" s="64">
         <v>7</v>
       </c>
-      <c r="L14" s="68">
+      <c r="L14" s="66">
         <v>7</v>
       </c>
-      <c r="M14" s="70" t="s">
-        <v>258</v>
-      </c>
-      <c r="N14" s="71" t="s">
-        <v>260</v>
-      </c>
-      <c r="O14" s="66">
+      <c r="M14" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="N14" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="O14" s="64">
         <v>7</v>
       </c>
-      <c r="P14" s="68">
+      <c r="P14" s="66">
         <v>8</v>
       </c>
-      <c r="Q14" s="74">
+      <c r="Q14" s="72">
         <v>6</v>
       </c>
-      <c r="R14" s="75">
+      <c r="R14" s="73">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.25">
       <c r="B15" s="48"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="83">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="81">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="G15" s="66" t="s">
-        <v>244</v>
-      </c>
-      <c r="H15" s="68" t="s">
-        <v>245</v>
-      </c>
-      <c r="I15" s="66" t="s">
-        <v>244</v>
-      </c>
-      <c r="J15" s="68" t="s">
-        <v>252</v>
-      </c>
-      <c r="K15" s="66">
+      <c r="G15" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="H15" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="K15" s="64">
         <v>7</v>
       </c>
-      <c r="L15" s="68">
+      <c r="L15" s="66">
         <v>7</v>
       </c>
-      <c r="M15" s="70" t="s">
-        <v>258</v>
-      </c>
-      <c r="N15" s="71" t="s">
-        <v>260</v>
-      </c>
-      <c r="O15" s="66">
+      <c r="M15" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="N15" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="O15" s="64">
         <v>7</v>
       </c>
-      <c r="P15" s="68">
+      <c r="P15" s="66">
         <v>8</v>
       </c>
-      <c r="Q15" s="74">
+      <c r="Q15" s="72">
         <v>7</v>
       </c>
-      <c r="R15" s="75">
+      <c r="R15" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="14.25">
       <c r="B16" s="48"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="83">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="F16" s="85">
+      <c r="F16" s="81">
         <f t="shared" si="1"/>
         <v>7.1111111111111116</v>
       </c>
-      <c r="G16" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="H16" s="68">
+      <c r="G16" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" s="66">
         <v>8</v>
       </c>
-      <c r="I16" s="66" t="s">
-        <v>253</v>
-      </c>
-      <c r="J16" s="68">
+      <c r="I16" s="64" t="s">
+        <v>249</v>
+      </c>
+      <c r="J16" s="66">
         <v>7</v>
       </c>
-      <c r="K16" s="66">
+      <c r="K16" s="64">
         <v>7</v>
       </c>
-      <c r="L16" s="68">
+      <c r="L16" s="66">
         <v>7</v>
       </c>
-      <c r="M16" s="70" t="s">
-        <v>261</v>
-      </c>
-      <c r="N16" s="71" t="s">
-        <v>262</v>
-      </c>
-      <c r="O16" s="66">
+      <c r="M16" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="N16" s="69" t="s">
+        <v>258</v>
+      </c>
+      <c r="O16" s="64">
         <v>7</v>
       </c>
-      <c r="P16" s="68">
+      <c r="P16" s="66">
         <v>8</v>
       </c>
-      <c r="Q16" s="74">
+      <c r="Q16" s="72">
         <v>6</v>
       </c>
-      <c r="R16" s="75">
+      <c r="R16" s="73">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="14.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="94" t="s">
+      <c r="C17" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="87">
+      <c r="D17" s="49"/>
+      <c r="E17" s="83">
         <f t="shared" si="0"/>
         <v>7.666666666666667</v>
       </c>
-      <c r="F17" s="96">
+      <c r="F17" s="92">
         <f t="shared" si="1"/>
         <v>7.7777777777777786</v>
       </c>
-      <c r="G17" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="H17" s="68">
+      <c r="G17" s="64" t="s">
+        <v>242</v>
+      </c>
+      <c r="H17" s="66">
         <v>7</v>
       </c>
-      <c r="I17" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="J17" s="68">
+      <c r="I17" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" s="66">
         <v>8</v>
       </c>
-      <c r="K17" s="66">
+      <c r="K17" s="64">
         <v>8</v>
       </c>
-      <c r="L17" s="68">
+      <c r="L17" s="66">
         <v>8</v>
       </c>
-      <c r="M17" s="70" t="s">
-        <v>263</v>
-      </c>
-      <c r="N17" s="71" t="s">
-        <v>264</v>
-      </c>
-      <c r="O17" s="66">
+      <c r="M17" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="N17" s="69" t="s">
+        <v>260</v>
+      </c>
+      <c r="O17" s="64">
         <v>9</v>
       </c>
-      <c r="P17" s="68">
+      <c r="P17" s="66">
         <v>8</v>
       </c>
-      <c r="Q17" s="74">
+      <c r="Q17" s="72">
         <v>6</v>
       </c>
-      <c r="R17" s="75">
+      <c r="R17" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="14.25">
       <c r="B18" s="48"/>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="87">
+      <c r="D18" s="49"/>
+      <c r="E18" s="83">
         <f t="shared" si="0"/>
         <v>7.666666666666667</v>
       </c>
-      <c r="F18" s="96">
+      <c r="F18" s="92">
         <f t="shared" si="1"/>
         <v>7.916666666666667</v>
       </c>
-      <c r="G18" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="H18" s="68" t="s">
-        <v>247</v>
-      </c>
-      <c r="I18" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="J18" s="68" t="s">
-        <v>254</v>
-      </c>
-      <c r="K18" s="66">
+      <c r="G18" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H18" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="I18" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="J18" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="K18" s="64">
         <v>8</v>
       </c>
-      <c r="L18" s="68">
+      <c r="L18" s="66">
         <v>8</v>
       </c>
-      <c r="M18" s="70" t="s">
-        <v>263</v>
-      </c>
-      <c r="N18" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="O18" s="66">
+      <c r="M18" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="N18" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="O18" s="64">
         <v>9</v>
       </c>
-      <c r="P18" s="68">
+      <c r="P18" s="66">
         <v>8</v>
       </c>
-      <c r="Q18" s="74">
+      <c r="Q18" s="72">
         <v>6</v>
       </c>
-      <c r="R18" s="75">
+      <c r="R18" s="73">
         <v>8</v>
       </c>
     </row>
@@ -6637,49 +7152,49 @@
         <v>187</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="87">
+      <c r="D19" s="49"/>
+      <c r="E19" s="83">
         <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="81">
         <f t="shared" si="1"/>
         <v>6.4761904761904754</v>
       </c>
-      <c r="G19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="H19" s="68">
+      <c r="G19" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="H19" s="66">
         <v>7</v>
       </c>
-      <c r="I19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="J19" s="68">
+      <c r="I19" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19" s="66">
         <v>6</v>
       </c>
-      <c r="K19" s="66">
+      <c r="K19" s="64">
         <v>6</v>
       </c>
-      <c r="L19" s="68">
+      <c r="L19" s="66">
         <v>6</v>
       </c>
-      <c r="M19" s="70" t="s">
-        <v>261</v>
-      </c>
-      <c r="N19" s="68">
+      <c r="M19" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="N19" s="66">
         <v>4</v>
       </c>
-      <c r="O19" s="66">
+      <c r="O19" s="64">
         <v>8</v>
       </c>
-      <c r="P19" s="68">
+      <c r="P19" s="66">
         <v>9</v>
       </c>
-      <c r="Q19" s="74">
+      <c r="Q19" s="72">
         <v>5</v>
       </c>
-      <c r="R19" s="75">
+      <c r="R19" s="73">
         <v>7</v>
       </c>
     </row>
@@ -6690,49 +7205,49 @@
       <c r="C20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="87">
+      <c r="D20" s="49"/>
+      <c r="E20" s="83">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="F20" s="85">
+      <c r="F20" s="81">
         <f t="shared" si="1"/>
         <v>5.3888888888888884</v>
       </c>
-      <c r="G20" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="H20" s="68">
+      <c r="G20" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="H20" s="66">
         <v>5</v>
       </c>
-      <c r="I20" s="66" t="s">
-        <v>255</v>
-      </c>
-      <c r="J20" s="68">
+      <c r="I20" s="64" t="s">
+        <v>251</v>
+      </c>
+      <c r="J20" s="66">
         <v>2</v>
       </c>
-      <c r="K20" s="66">
+      <c r="K20" s="64">
         <v>7</v>
       </c>
-      <c r="L20" s="68">
+      <c r="L20" s="66">
         <v>7</v>
       </c>
-      <c r="M20" s="70" t="s">
-        <v>266</v>
-      </c>
-      <c r="N20" s="71" t="s">
-        <v>267</v>
-      </c>
-      <c r="O20" s="66">
+      <c r="M20" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="N20" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="O20" s="64">
         <v>4</v>
       </c>
-      <c r="P20" s="68">
+      <c r="P20" s="66">
         <v>7</v>
       </c>
-      <c r="Q20" s="74">
+      <c r="Q20" s="72">
         <v>5</v>
       </c>
-      <c r="R20" s="75">
+      <c r="R20" s="73">
         <v>6</v>
       </c>
     </row>
@@ -6741,49 +7256,49 @@
       <c r="C21" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="87">
+      <c r="D21" s="49"/>
+      <c r="E21" s="83">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F21" s="85">
+      <c r="F21" s="81">
         <f t="shared" si="1"/>
         <v>5.833333333333333</v>
       </c>
-      <c r="G21" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="H21" s="68">
+      <c r="G21" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="H21" s="66">
         <v>5</v>
       </c>
-      <c r="I21" s="66" t="s">
-        <v>255</v>
-      </c>
-      <c r="J21" s="68">
+      <c r="I21" s="64" t="s">
+        <v>251</v>
+      </c>
+      <c r="J21" s="66">
         <v>2</v>
       </c>
-      <c r="K21" s="66">
+      <c r="K21" s="64">
         <v>7</v>
       </c>
-      <c r="L21" s="68">
+      <c r="L21" s="66">
         <v>7</v>
       </c>
-      <c r="M21" s="70" t="s">
-        <v>266</v>
-      </c>
-      <c r="N21" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="O21" s="66">
+      <c r="M21" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="N21" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="O21" s="64">
         <v>5</v>
       </c>
-      <c r="P21" s="68">
+      <c r="P21" s="66">
         <v>7</v>
       </c>
-      <c r="Q21" s="74">
+      <c r="Q21" s="72">
         <v>6</v>
       </c>
-      <c r="R21" s="75">
+      <c r="R21" s="73">
         <v>8</v>
       </c>
     </row>
@@ -6792,49 +7307,49 @@
         <v>189</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="87">
+      <c r="D22" s="49"/>
+      <c r="E22" s="83">
         <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="F22" s="85">
+      <c r="F22" s="81">
         <f t="shared" si="1"/>
         <v>6.7222222222222214</v>
       </c>
-      <c r="G22" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="H22" s="68">
+      <c r="G22" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H22" s="66">
         <v>7</v>
       </c>
-      <c r="I22" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="J22" s="68">
+      <c r="I22" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="J22" s="66">
         <v>7</v>
       </c>
-      <c r="K22" s="66">
+      <c r="K22" s="64">
         <v>8</v>
       </c>
-      <c r="L22" s="68">
+      <c r="L22" s="66">
         <v>8</v>
       </c>
-      <c r="M22" s="70" t="s">
-        <v>261</v>
-      </c>
-      <c r="N22" s="71" t="s">
-        <v>269</v>
-      </c>
-      <c r="O22" s="66">
+      <c r="M22" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="N22" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="O22" s="64">
         <v>6</v>
       </c>
-      <c r="P22" s="68">
+      <c r="P22" s="66">
         <v>4</v>
       </c>
-      <c r="Q22" s="74">
+      <c r="Q22" s="72">
         <v>5</v>
       </c>
-      <c r="R22" s="75">
+      <c r="R22" s="73">
         <v>8</v>
       </c>
     </row>
@@ -6843,49 +7358,49 @@
         <v>190</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="87">
+      <c r="D23" s="49"/>
+      <c r="E23" s="83">
         <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="F23" s="85">
+      <c r="F23" s="81">
         <f t="shared" si="1"/>
         <v>5.3888888888888884</v>
       </c>
-      <c r="G23" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="H23" s="68">
+      <c r="G23" s="64" t="s">
+        <v>242</v>
+      </c>
+      <c r="H23" s="66">
         <v>3</v>
       </c>
-      <c r="I23" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="J23" s="68">
+      <c r="I23" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="J23" s="66">
         <v>3</v>
       </c>
-      <c r="K23" s="66">
+      <c r="K23" s="64">
         <v>6</v>
       </c>
-      <c r="L23" s="68">
+      <c r="L23" s="66">
         <v>6</v>
       </c>
-      <c r="M23" s="70" t="s">
+      <c r="M23" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="N23" s="69" t="s">
         <v>263</v>
       </c>
-      <c r="N23" s="71" t="s">
-        <v>267</v>
-      </c>
-      <c r="O23" s="66">
+      <c r="O23" s="64">
         <v>8</v>
       </c>
-      <c r="P23" s="68">
+      <c r="P23" s="66">
         <v>6</v>
       </c>
-      <c r="Q23" s="74">
+      <c r="Q23" s="72">
         <v>5</v>
       </c>
-      <c r="R23" s="75">
+      <c r="R23" s="73">
         <v>8</v>
       </c>
     </row>
@@ -6894,111 +7409,111 @@
         <v>191</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="87">
+      <c r="D24" s="49"/>
+      <c r="E24" s="83">
         <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="F24" s="85">
+      <c r="F24" s="81">
         <f t="shared" si="1"/>
         <v>4.7222222222222223</v>
       </c>
-      <c r="G24" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="H24" s="68">
+      <c r="G24" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H24" s="66">
         <v>4</v>
       </c>
-      <c r="I24" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="J24" s="68">
+      <c r="I24" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="J24" s="66">
         <v>4</v>
       </c>
-      <c r="K24" s="66">
+      <c r="K24" s="64">
         <v>4</v>
       </c>
-      <c r="L24" s="68">
+      <c r="L24" s="66">
         <v>4</v>
       </c>
-      <c r="M24" s="70" t="s">
-        <v>270</v>
-      </c>
-      <c r="N24" s="71" t="s">
-        <v>271</v>
-      </c>
-      <c r="O24" s="66">
+      <c r="M24" s="68" t="s">
+        <v>266</v>
+      </c>
+      <c r="N24" s="69" t="s">
+        <v>267</v>
+      </c>
+      <c r="O24" s="64">
         <v>3</v>
       </c>
-      <c r="P24" s="68">
+      <c r="P24" s="66">
         <v>5</v>
       </c>
-      <c r="Q24" s="74">
+      <c r="Q24" s="72">
         <v>6</v>
       </c>
-      <c r="R24" s="75">
+      <c r="R24" s="73">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" thickBot="1">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="88">
+      <c r="C25" s="50"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="84">
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
-      <c r="F25" s="86">
+      <c r="F25" s="82">
         <f t="shared" si="1"/>
         <v>4.625</v>
       </c>
-      <c r="G25" s="67" t="s">
-        <v>249</v>
-      </c>
-      <c r="H25" s="69">
+      <c r="G25" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="H25" s="67">
         <v>4</v>
       </c>
-      <c r="I25" s="67">
+      <c r="I25" s="65">
         <v>7</v>
       </c>
-      <c r="J25" s="69">
+      <c r="J25" s="67">
         <v>4</v>
       </c>
-      <c r="K25" s="67">
+      <c r="K25" s="65">
         <v>5</v>
       </c>
-      <c r="L25" s="69">
+      <c r="L25" s="67">
         <v>5</v>
       </c>
-      <c r="M25" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="N25" s="73" t="s">
-        <v>272</v>
-      </c>
-      <c r="O25" s="67">
+      <c r="M25" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="N25" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="O25" s="65">
         <v>2</v>
       </c>
-      <c r="P25" s="69">
+      <c r="P25" s="67">
         <v>3</v>
       </c>
-      <c r="Q25" s="76">
+      <c r="Q25" s="74">
         <v>5</v>
       </c>
-      <c r="R25" s="77">
+      <c r="R25" s="75">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="14.25" thickBot="1">
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="108"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="109"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="119"/>
     </row>
   </sheetData>
   <autoFilter ref="B11:F11"/>
@@ -7016,7 +7531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J12"/>
   <sheetViews>
@@ -7034,273 +7549,273 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="31.5">
-      <c r="B2" s="89" t="s">
-        <v>319</v>
-      </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="85" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
     </row>
     <row r="3" spans="2:10" ht="14.25" thickBot="1">
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
     </row>
     <row r="4" spans="2:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B4" s="97" t="s">
-        <v>279</v>
-      </c>
-      <c r="C4" s="98" t="s">
-        <v>321</v>
-      </c>
-      <c r="D4" s="99" t="s">
-        <v>322</v>
-      </c>
-      <c r="E4" s="135" t="s">
-        <v>320</v>
-      </c>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="137"/>
+      <c r="B4" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="95" t="s">
+        <v>307</v>
+      </c>
+      <c r="E4" s="145" t="s">
+        <v>305</v>
+      </c>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="147"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1">
-      <c r="B5" s="81" t="s">
-        <v>280</v>
-      </c>
-      <c r="C5" s="91">
+      <c r="B5" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="87">
         <f t="shared" ref="C5:C12" si="0">AVERAGE(E5:J5)</f>
         <v>6.333333333333333</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="82">
+      <c r="E5" s="80">
         <v>3</v>
       </c>
-      <c r="F5" s="82">
+      <c r="F5" s="80">
         <v>8</v>
       </c>
-      <c r="G5" s="82">
+      <c r="G5" s="80">
         <v>8</v>
       </c>
-      <c r="H5" s="82">
+      <c r="H5" s="80">
         <v>8</v>
       </c>
-      <c r="I5" s="82">
+      <c r="I5" s="80">
         <v>8</v>
       </c>
-      <c r="J5" s="82">
+      <c r="J5" s="80">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" thickBot="1">
-      <c r="B6" s="81" t="s">
-        <v>324</v>
-      </c>
-      <c r="C6" s="93">
+      <c r="B6" s="79" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" s="89">
         <f t="shared" si="0"/>
         <v>7.833333333333333</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="82">
+      <c r="E6" s="80">
         <v>7</v>
       </c>
-      <c r="F6" s="82">
+      <c r="F6" s="80">
         <v>7</v>
       </c>
-      <c r="G6" s="82">
+      <c r="G6" s="80">
         <v>8</v>
       </c>
-      <c r="H6" s="82">
+      <c r="H6" s="80">
         <v>8</v>
       </c>
-      <c r="I6" s="82">
+      <c r="I6" s="80">
         <v>8</v>
       </c>
-      <c r="J6" s="82">
+      <c r="J6" s="80">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1">
-      <c r="B7" s="81" t="s">
-        <v>323</v>
-      </c>
-      <c r="C7" s="91">
+      <c r="B7" s="79" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" s="87">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="82">
+      <c r="E7" s="80">
         <v>6</v>
       </c>
-      <c r="F7" s="82">
+      <c r="F7" s="80">
         <v>9</v>
       </c>
-      <c r="G7" s="82">
+      <c r="G7" s="80">
         <v>6</v>
       </c>
-      <c r="H7" s="82">
+      <c r="H7" s="80">
         <v>5</v>
       </c>
-      <c r="I7" s="82">
+      <c r="I7" s="80">
         <v>6</v>
       </c>
-      <c r="J7" s="82">
+      <c r="J7" s="80">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" thickBot="1">
-      <c r="B8" s="81" t="s">
-        <v>281</v>
-      </c>
-      <c r="C8" s="91">
+      <c r="B8" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="87">
         <f t="shared" si="0"/>
         <v>7.166666666666667</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="E8" s="82">
+      <c r="E8" s="80">
         <v>8</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="80">
         <v>7</v>
       </c>
-      <c r="G8" s="82">
+      <c r="G8" s="80">
         <v>7</v>
       </c>
-      <c r="H8" s="82">
+      <c r="H8" s="80">
         <v>6</v>
       </c>
-      <c r="I8" s="82">
+      <c r="I8" s="80">
         <v>7</v>
       </c>
-      <c r="J8" s="82">
+      <c r="J8" s="80">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1">
-      <c r="B9" s="81" t="s">
-        <v>282</v>
-      </c>
-      <c r="C9" s="91">
+      <c r="B9" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" s="87">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="82">
+      <c r="E9" s="80">
         <v>6</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="80">
         <v>8</v>
       </c>
-      <c r="G9" s="82">
+      <c r="G9" s="80">
         <v>8</v>
       </c>
-      <c r="H9" s="82">
+      <c r="H9" s="80">
         <v>7</v>
       </c>
-      <c r="I9" s="82">
+      <c r="I9" s="80">
         <v>9</v>
       </c>
-      <c r="J9" s="82">
+      <c r="J9" s="80">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" thickBot="1">
-      <c r="B10" s="81" t="s">
-        <v>325</v>
-      </c>
-      <c r="C10" s="91">
+      <c r="B10" s="79" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="87">
         <f t="shared" si="0"/>
         <v>7.333333333333333</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="88" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="82">
+      <c r="E10" s="80">
         <v>6</v>
       </c>
-      <c r="F10" s="82">
+      <c r="F10" s="80">
         <v>9</v>
       </c>
-      <c r="G10" s="82">
+      <c r="G10" s="80">
         <v>9</v>
       </c>
-      <c r="H10" s="82">
+      <c r="H10" s="80">
         <v>7</v>
       </c>
-      <c r="I10" s="82">
+      <c r="I10" s="80">
         <v>8</v>
       </c>
-      <c r="J10" s="82">
+      <c r="J10" s="80">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1">
-      <c r="B11" s="81" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" s="91">
+      <c r="B11" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="87">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="80">
         <v>7</v>
       </c>
-      <c r="F11" s="82">
+      <c r="F11" s="80">
         <v>5</v>
       </c>
-      <c r="G11" s="82">
+      <c r="G11" s="80">
         <v>8</v>
       </c>
-      <c r="H11" s="82">
+      <c r="H11" s="80">
         <v>7</v>
       </c>
-      <c r="I11" s="82">
+      <c r="I11" s="80">
         <v>8</v>
       </c>
-      <c r="J11" s="82">
+      <c r="J11" s="80">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1">
-      <c r="B12" s="81" t="s">
-        <v>284</v>
-      </c>
-      <c r="C12" s="91">
+      <c r="B12" s="79" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="87">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D12" s="92" t="s">
-        <v>211</v>
-      </c>
-      <c r="E12" s="82">
+      <c r="D12" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="80">
         <v>7</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="80">
         <v>5</v>
       </c>
-      <c r="G12" s="82">
+      <c r="G12" s="80">
         <v>7</v>
       </c>
-      <c r="H12" s="82">
+      <c r="H12" s="80">
         <v>7</v>
       </c>
-      <c r="I12" s="82">
+      <c r="I12" s="80">
         <v>9</v>
       </c>
-      <c r="J12" s="82">
+      <c r="J12" s="80">
         <v>7</v>
       </c>
     </row>
@@ -7508,10 +8023,10 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -7519,8 +8034,8 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="75" customHeight="1">
-      <c r="B9" s="102"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -7528,8 +8043,8 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1">
-      <c r="B10" s="102"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -7537,8 +8052,8 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" thickBot="1">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -7747,10 +8262,10 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -7758,8 +8273,8 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="75" customHeight="1">
-      <c r="B9" s="102"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -7767,8 +8282,8 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1">
-      <c r="B10" s="102"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -7776,8 +8291,8 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" thickBot="1">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -7840,10 +8355,10 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="110" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -7851,8 +8366,8 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="75" customHeight="1">
-      <c r="B9" s="102"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -7860,8 +8375,8 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1">
-      <c r="B10" s="102"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -7869,8 +8384,8 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" thickBot="1">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -7933,10 +8448,10 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="110" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -7944,8 +8459,8 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="75" customHeight="1">
-      <c r="B9" s="102"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -7953,8 +8468,8 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1">
-      <c r="B10" s="102"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -7962,8 +8477,8 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" thickBot="1">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>

</xml_diff>